<commit_message>
Updated Missing Data code, minor updates to Habitat_Data_Raw (Data Sources), minor Tier 1 script updates
Missing Data was to update to include both HQ metrics and core metrics, and only have output be one column.

Tier 1 script was updated to be able to select with tier 1 - species to choose.
</commit_message>
<xml_diff>
--- a/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,7 +425,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook</t>
+          <t>HQ_spring_chinook,LF_spring_chinook</t>
         </is>
       </c>
       <c r="E6">
@@ -560,12 +560,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -595,12 +595,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook</t>
+          <t>HQ_spring_chinook,LF_spring_chinook</t>
         </is>
       </c>
       <c r="E8">
@@ -630,12 +630,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -694,12 +694,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -729,12 +729,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -791,20 +791,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,HQ_steelhead,LF_spring_chinook,LF_steelhead</t>
+          <t>HQ_spring_chinook,HQ_steelhead</t>
         </is>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -826,20 +826,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,HQ_steelhead,LF_spring_chinook,LF_steelhead</t>
+          <t>HQ_spring_chinook,HQ_steelhead</t>
         </is>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -861,20 +861,20 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,HQ_steelhead,LF_spring_chinook,LF_steelhead</t>
+          <t>HQ_spring_chinook,HQ_steelhead</t>
         </is>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -896,20 +896,20 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,HQ_steelhead,LF_spring_chinook,LF_steelhead</t>
+          <t>HQ_spring_chinook,HQ_steelhead,LF_steelhead</t>
         </is>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
@@ -931,20 +931,20 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,LF_spring_chinook</t>
+          <t>HQ_spring_chinook</t>
         </is>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -966,20 +966,20 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,LF_spring_chinook</t>
+          <t>HQ_spring_chinook</t>
         </is>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1176,20 +1176,20 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>HQ_spring_chinook,HQ_steelhead,LF_spring_chinook,LF_steelhead</t>
+          <t>HQ_spring_chinook,HQ_steelhead</t>
         </is>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1289,12 +1289,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1324,12 +1324,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1673,14 +1673,14 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 02</t>
+          <t>Little Wenatchee River Lower 01</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1698,17 +1698,14 @@
           <t>LF_spring_chinook</t>
         </is>
       </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
@@ -1738,12 +1735,12 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1773,12 +1770,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
@@ -1805,19 +1802,19 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 04</t>
+          <t>Nason Creek Lower 15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1840,34 +1837,34 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Holding and Maturation,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 05</t>
+          <t>Chewuch River Pearrygin 10</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Chewuch River-Pearrygin Creek</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
+          <t>LF_spring_chinook</t>
         </is>
       </c>
       <c r="E44">
@@ -1875,19 +1872,19 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 06</t>
+          <t>Chiwawa River Middle 04</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1897,67 +1894,61 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Middle Chiwawa River</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E45">
-        <v>3</v>
+          <t>LF_spring_chinook</t>
+        </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 07</t>
+          <t>Entiat River Potato 04</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E46">
-        <v>3</v>
+          <t>LF_spring_chinook</t>
+        </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 08</t>
+          <t>Nason Creek Lower 05</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1976,33 +1967,33 @@
         </is>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Smolt Outmigration,Spawning and Incubation,Winter Rearing</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 10</t>
+          <t>Twisp River Middle 07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Middle Twisp River</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2011,42 +2002,42 @@
         </is>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Smolt Outmigration,Winter Rearing,Summer Rearing</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 11</t>
+          <t>Entiat River Lake 02</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
+          <t>LF_spring_chinook</t>
         </is>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2055,33 +2046,30 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 12</t>
+          <t>Entiat River Lake 11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E50">
-        <v>3</v>
+          <t>LF_spring_chinook</t>
+        </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2090,14 +2078,14 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 13</t>
+          <t>Little Wenatchee River Lower 02</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2107,12 +2095,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Little Wenatchee River</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
+          <t>LF_spring_chinook</t>
         </is>
       </c>
       <c r="E51">
@@ -2125,14 +2113,14 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 14</t>
+          <t>Nason Creek Lower 04</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2151,7 +2139,7 @@
         </is>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2160,14 +2148,14 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 15</t>
+          <t>Nason Creek Lower 06</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2190,19 +2178,19 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>White River Lower 05</t>
+          <t>Nason Creek Lower 07</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2212,13 +2200,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Lower White River</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_bull_trout</t>
-        </is>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
+      </c>
+      <c r="E54">
+        <v>3</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2227,199 +2218,184 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Chewuch River Pearrygin 01</t>
+          <t>Nason Creek Lower 08</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Chewuch River-Pearrygin Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E55">
-        <v>1</v>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Chewuch River Pearrygin 02</t>
+          <t>Nason Creek Lower 10</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Chewuch River-Pearrygin Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E56">
-        <v>3</v>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Chewuch River Pearrygin 03</t>
+          <t>Nason Creek Lower 11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Chewuch River-Pearrygin Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E57">
-        <v>1</v>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Entiat River Preston 03</t>
+          <t>Nason Creek Lower 12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E58">
-        <v>3</v>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Entiat River Preston 04</t>
+          <t>Nason Creek Lower 13</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E59">
-        <v>3</v>
+          <t>LF_spring_chinook,LF_steelhead</t>
+        </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Stormy Creek 01</t>
+          <t>Nason Creek Lower 14</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2429,19 +2405,19 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Chiwawa River Lower 07</t>
+          <t>White River Lower 05</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2451,243 +2427,231 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Lower Chiwawa River</t>
+          <t>Lower White River</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
-        </is>
-      </c>
-      <c r="E61">
-        <v>3</v>
+          <t>LF_spring_chinook,LF_bull_trout</t>
+        </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Entiat River Potato 01</t>
+          <t>Chewuch River Doe 08</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Chewuch River-Doe Creek</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
+          <t>LF_spring_chinook</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Entiat River Potato 03</t>
+          <t>Icicle Creek Lower 06</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Lower Icicle Creek</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
+          <t>LF_steelhead</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Entiat River Preston 01</t>
+          <t>Icicle Creek Lower 07</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Lower Icicle Creek</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>LF_spring_chinook</t>
+          <t>LF_steelhead</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Methow River Thompson 03</t>
+          <t>Nason Creek Lower 09</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Methow River-Thompson Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E65">
-        <v>3</v>
+          <t>LF_steelhead</t>
+        </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Methow River Thompson 05</t>
+          <t>Antoine 16-1</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Methow River-Thompson Creek</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E66">
-        <v>1</v>
+          <t>LF_steelhead</t>
+        </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Methow River Thompson 06</t>
+          <t>Antoine 16-2</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Methow River-Thompson Creek</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>LF_spring_chinook,LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E67">
-        <v>3</v>
+          <t>LF_steelhead</t>
+        </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 09</t>
+          <t>Antoine 16-3</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2695,34 +2659,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E68">
-        <v>3</v>
-      </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Entiat River Mills 02</t>
+          <t>Antoine 16-5</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2730,34 +2691,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E69">
-        <v>3</v>
-      </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Entiat River Mills 03</t>
+          <t>Antoine 16-6</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2765,34 +2723,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E70">
-        <v>3</v>
-      </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Entiat River Mills 04</t>
+          <t>Bonaparte 16-1</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Bonaparte Creek-Lower DS</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2800,34 +2755,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Entiat River Mills 05</t>
+          <t>Loup Loup 16-1</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2835,34 +2787,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Entiat River Mills 06</t>
+          <t>Loup Loup 16-2</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2870,34 +2819,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E73">
-        <v>3</v>
-      </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Entiat River Mills 07</t>
+          <t>Loup Loup 16-3</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2907,29 +2853,29 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Entiat River Mills 08</t>
+          <t>Salmon 16-10</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Entiat River-Mills Creek</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2937,31 +2883,34 @@
           <t>LF_steelhead</t>
         </is>
       </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Twisp River Lower 02</t>
+          <t>Salmon 16-12</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2969,34 +2918,31 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E76">
-        <v>3</v>
-      </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Twisp River Lower 03</t>
+          <t>Salmon 16-2</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3006,29 +2952,29 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Twisp River Lower 04</t>
+          <t>Salmon 16-4</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3036,31 +2982,34 @@
           <t>LF_steelhead</t>
         </is>
       </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Twisp River Lower 05</t>
+          <t>Salmon 16-8</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3073,29 +3022,29 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Twisp River Lower 07</t>
+          <t>Similkameen 16-2</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Similkameen River</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3105,29 +3054,29 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Twisp River Lower 08</t>
+          <t>Similkameen 16-3</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Similkameen River</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3135,31 +3084,34 @@
           <t>LF_steelhead</t>
         </is>
       </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Twisp River Lower 10</t>
+          <t>Similkameen 16-6</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Lower Twisp River</t>
+          <t>Similkameen River</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3169,19 +3121,19 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Antoine 16-1</t>
+          <t>Omak 16-2</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3191,7 +3143,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Omak Creek-Lower DS</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3199,24 +3151,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E83">
-        <v>3</v>
-      </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Summer Rearing</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Antoine 16-2</t>
+          <t>Omak 16-3</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3226,7 +3175,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Omak Creek-Lower DS</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3236,19 +3185,19 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Summer Rearing</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Antoine 16-3</t>
+          <t>Omak 16-5</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3258,7 +3207,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3266,24 +3215,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E85">
-        <v>2</v>
-      </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Summer Rearing</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Antoine 16-5</t>
+          <t>Omak 16-1</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3293,7 +3239,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Omak Creek-Lower DS</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3301,24 +3247,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E86">
-        <v>1</v>
-      </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Antoine 16-6</t>
+          <t>Omak 16-6</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3328,7 +3271,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3336,24 +3279,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E87">
-        <v>2</v>
-      </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Bonaparte 16-1</t>
+          <t>Omak 16-7</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3363,7 +3303,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Bonaparte Creek-Lower DS</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3373,19 +3313,19 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Loup Loup 16-1</t>
+          <t>Omak 16-8</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3395,7 +3335,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3403,24 +3343,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E89">
-        <v>3</v>
-      </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Loup Loup 16-2</t>
+          <t>Omak 16-9</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3430,7 +3367,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3438,24 +3375,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E90">
-        <v>1</v>
-      </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Loup Loup 16-3</t>
+          <t>Salmon 16-3</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3465,7 +3399,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3473,24 +3407,21 @@
           <t>LF_steelhead</t>
         </is>
       </c>
-      <c r="E91">
-        <v>2</v>
-      </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Salmon 16-10</t>
+          <t>Salmon 16-7</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3509,344 +3440,326 @@
         </is>
       </c>
       <c r="E92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Salmon 16-12</t>
+          <t>Cougar Creek 01</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
+          <t>LF_bull_trout</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Salmon 16-2</t>
+          <t>Mad River Upper 01</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
+          <t>LF_bull_trout</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Salmon 16-4</t>
+          <t>Mad River Upper 02</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E95">
-        <v>3</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Salmon 16-8</t>
+          <t>Mad River Upper 03</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E96">
-        <v>3</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Similkameen 16-2</t>
+          <t>Mad River Upper 04</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E97">
-        <v>3</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Similkameen 16-3</t>
+          <t>Mad River Upper 05</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Upper Mad River</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E98">
-        <v>3</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Adult Migration</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Similkameen 16-6</t>
+          <t>Chikamin Creek 01</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Chikamin Creek</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
+          <t>LF_bull_trout</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Omak 16-2</t>
+          <t>Chikamin Creek 03</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Chikamin Creek</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E100">
-        <v>3</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Omak 16-3</t>
+          <t>Chiwaukum Creek 02</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Chiwaukum Creek</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E101">
-        <v>1</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Omak 16-5</t>
+          <t>Twisp River Upper 01</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Upper Twisp River</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
+          <t>LF_bull_trout</t>
         </is>
       </c>
       <c r="E102">
@@ -3854,289 +3767,76 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Omak 16-1</t>
+          <t>Twisp River Upper 02</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Upper Twisp River</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E103">
-        <v>2</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Omak 16-6</t>
+          <t>Twisp River Upper 03</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Upper Twisp River</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E104">
-        <v>2</v>
+          <t>LF_bull_trout</t>
+        </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>Omak 16-7</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Okanogan</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Omak Creek-Lower US</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Summer Rearing</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Omak 16-8</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Okanogan</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Omak Creek-Lower US</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E106">
-        <v>1</v>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Summer Rearing</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Omak 16-9</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Okanogan</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Omak Creek-Lower US</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E107">
-        <v>2</v>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Summer Rearing</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>Salmon 16-3</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Okanogan</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Salmon Creek-Lower</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Summer Rearing</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>Salmon 16-7</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Okanogan</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Salmon Creek-Lower</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>LF_steelhead</t>
-        </is>
-      </c>
-      <c r="E109">
-        <v>1</v>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Summer Rearing</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Mad River Upper 02</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Entiat</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Upper Mad River</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>LF_bull_trout</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Adult Non-Spawning</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>Habitat Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update so MASTER is read in directly
Also allows for MASTER data tabs to be saved, and those excel files read in (instead of straight from the MASTER).
</commit_message>
<xml_diff>
--- a/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -883,7 +883,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Summer Rearing,Winter Rearing</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Adult Migration,Smolt Outmigration,Spawning and Incubation</t>
+          <t>Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1958,17 +1958,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Methow River Thompson 01</t>
+          <t>Nason Creek Lower 04</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Methow River-Thompson Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1978,12 +1978,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Smolt Outmigration</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1995,7 +1995,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 04</t>
+          <t>Nason Creek Lower 05</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Spawning and Incubation,Winter Rearing</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2032,7 +2032,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 05</t>
+          <t>Nason Creek Lower 06</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2069,7 +2069,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 06</t>
+          <t>Nason Creek Lower 07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2106,7 +2106,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 07</t>
+          <t>Nason Creek Lower 15</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2143,17 +2143,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 15</t>
+          <t>Twisp River Middle 07</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Middle Twisp River</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2168,29 +2168,29 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Smolt Outmigration</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Twisp River Middle 07</t>
+          <t>Antoine 16-1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Middle Twisp River</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2198,26 +2198,21 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Winter Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Antoine 16-1</t>
+          <t>Antoine 16-2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2242,14 +2237,14 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Antoine 16-2</t>
+          <t>Antoine 16-3</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2274,14 +2269,14 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Antoine 16-3</t>
+          <t>Antoine 16-5</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2306,14 +2301,14 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Antoine 16-5</t>
+          <t>Antoine 16-6</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2345,7 +2340,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Antoine 16-6</t>
+          <t>Bonaparte 16-1</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2355,7 +2350,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Bonaparte Creek-Lower DS</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2370,14 +2365,14 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Bonaparte 16-1</t>
+          <t>Loup Loup 16-1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2387,7 +2382,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bonaparte Creek-Lower DS</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2402,14 +2397,14 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Loup Loup 16-1</t>
+          <t>Loup Loup 16-2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2441,7 +2436,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Loup Loup 16-2</t>
+          <t>Loup Loup 16-3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2473,7 +2468,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Loup Loup 16-3</t>
+          <t>Salmon 16-10</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2483,7 +2478,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2491,6 +2486,11 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
@@ -2498,14 +2498,14 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Salmon 16-10</t>
+          <t>Salmon 16-12</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2521,11 +2521,6 @@
       <c r="D61" t="inlineStr">
         <is>
           <t>Prevent Limiting Factors</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2542,7 +2537,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Salmon 16-12</t>
+          <t>Salmon 16-2</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2567,14 +2562,14 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Salmon 16-2</t>
+          <t>Salmon 16-4</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2590,6 +2585,11 @@
       <c r="D63" t="inlineStr">
         <is>
           <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2606,7 +2606,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Salmon 16-4</t>
+          <t>Salmon 16-8</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2636,14 +2636,14 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Salmon 16-8</t>
+          <t>Similkameen 16-2</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2653,17 +2653,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Similkameen River</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>Prevent Limiting Factors</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2680,7 +2675,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Similkameen 16-2</t>
+          <t>Similkameen 16-3</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2696,6 +2691,11 @@
       <c r="D66" t="inlineStr">
         <is>
           <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2712,7 +2712,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Similkameen 16-3</t>
+          <t>Similkameen 16-6</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2730,11 +2730,6 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F67" t="inlineStr">
         <is>
           <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
@@ -2742,14 +2737,14 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Management</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Similkameen 16-6</t>
+          <t>Omak 16-2</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2759,7 +2754,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Omak Creek-Lower DS</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2769,19 +2764,19 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Holding and Maturation,Summer Rearing</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Protection</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Omak 16-2</t>
+          <t>Omak 16-3</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2813,7 +2808,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Omak 16-3</t>
+          <t>Omak 16-5</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2823,7 +2818,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2845,7 +2840,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Omak 16-5</t>
+          <t>Omak 16-1</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2855,7 +2850,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Omak Creek-Lower DS</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2865,7 +2860,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Summer Rearing</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2877,7 +2872,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Omak 16-1</t>
+          <t>Omak 16-6</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2887,7 +2882,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Omak Creek-Lower US</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2909,7 +2904,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Omak 16-6</t>
+          <t>Omak 16-7</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2941,7 +2936,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Omak 16-7</t>
+          <t>Omak 16-8</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2973,7 +2968,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Omak 16-8</t>
+          <t>Omak 16-9</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3005,7 +3000,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Omak 16-9</t>
+          <t>Salmon 16-3</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3015,7 +3010,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3037,7 +3032,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Salmon 16-3</t>
+          <t>Salmon 16-7</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3055,6 +3050,11 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr">
         <is>
           <t>Summer Rearing</t>
@@ -3062,24 +3062,24 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Management and Protection</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Salmon 16-7</t>
+          <t>Twisp River Upper 01</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Upper Twisp River</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3089,52 +3089,15 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Spawning and Incubation</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
-        <is>
-          <t>Management and Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Twisp River Upper 01</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Methow</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Upper Twisp River</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Prevent Limiting Factors</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Spawning and Incubation</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
         <is>
           <t>Management</t>
         </is>

</xml_diff>

<commit_message>
Misc updates to prepare to output to WebMap
</commit_message>
<xml_diff>
--- a/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Protection_Prioritization_Output_for_WebMap_Table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,7 +427,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -533,12 +533,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -570,12 +570,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -607,12 +607,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -644,19 +644,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Entiat River Lake 06</t>
+          <t>Entiat River Lake 08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -671,24 +671,29 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Entiat River Lake 07</t>
+          <t>Entiat River Lake 10</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -703,24 +708,29 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Entiat River Lake 08</t>
+          <t>Entiat River Potato 05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -730,7 +740,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Entiat River-Lake Creek</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -740,24 +750,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Entiat River Lake 10</t>
+          <t>Entiat River Potato 06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -767,7 +777,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Entiat River-Lake Creek</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -777,24 +787,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Adult Migration,Holding and Maturation,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Entiat River Potato 05</t>
+          <t>Entiat River Potato 08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -809,29 +819,29 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Entiat River Potato 06</t>
+          <t>Entiat River Preston 02</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -841,34 +851,34 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Entiat River Potato 08</t>
+          <t>Entiat River Preston 05</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -878,7 +888,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -888,34 +898,34 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Smolt Outmigration</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Entiat River Preston 02</t>
+          <t>Little Wenatchee River Lower 03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Lower Little Wenatchee River</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -925,7 +935,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -935,24 +945,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Entiat River Preston 05</t>
+          <t>Methow River Fawn 02</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Entiat River-Lake Creek</t>
+          <t>Methow River-Fawn Creek</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -962,7 +972,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -972,51 +982,51 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 03</t>
+          <t>Methow River Fawn 04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Lower Little Wenatchee River</t>
+          <t>Methow River-Fawn Creek</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Methow River Fawn 04</t>
+          <t>Methow River Rattlesnake 01</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1026,7 +1036,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Methow River-Fawn Creek</t>
+          <t>Methow River-Rattlesnake Creek</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1046,14 +1056,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Methow River Rattlesnake 01</t>
+          <t>Methow River Rattlesnake 05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1073,7 +1083,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1083,14 +1093,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Methow River Rattlesnake 05</t>
+          <t>Methow River Rattlesnake 06</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1120,14 +1130,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Methow River Rattlesnake 06</t>
+          <t>Methow River Thompson 07</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1137,34 +1147,34 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Methow River-Rattlesnake Creek</t>
+          <t>Methow River-Thompson Creek</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Methow River Thompson 07</t>
+          <t>Methow River Thompson 08</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1184,7 +1194,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1194,29 +1204,29 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Methow River Thompson 08</t>
+          <t>Nason Creek Lower 01</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Methow River-Thompson Creek</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1226,19 +1236,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 01</t>
+          <t>Nason Creek Lower 02</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1258,24 +1268,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 02</t>
+          <t>Nason Creek Lower 03</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1300,56 +1310,51 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 03</t>
+          <t>Twisp River Middle 01</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Middle Twisp River</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Twisp River Middle 01</t>
+          <t>Twisp River Middle 02</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1374,14 +1379,14 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Twisp River Middle 02</t>
+          <t>Twisp River Middle 06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1399,6 +1404,11 @@
           <t>Maintain Reach Function</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1406,24 +1416,24 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Twisp River Middle 06</t>
+          <t>White River Lower 08</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Middle Twisp River</t>
+          <t>Lower White River</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1443,14 +1453,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>White River Lower 08</t>
+          <t>Big Meadow Creek 01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1460,12 +1470,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lower White River</t>
+          <t>Big Meadow Creek</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1475,49 +1485,49 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Big Meadow Creek 01</t>
+          <t>Entiat River Mills 05</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Big Meadow Creek</t>
+          <t>Entiat River-Mills Creek</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Maintain Reach Function</t>
+          <t>Maintain Reach Function,Prevent Limiting Factors</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
@@ -1554,7 +1564,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1601,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1638,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1675,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1697,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1697,12 +1707,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
@@ -1724,7 +1734,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Maintain Reach Function,Prevent Limiting Factors</t>
+          <t>Maintain Reach Function</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1734,19 +1744,19 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Chewuch River Doe 08</t>
+          <t>Chewuch River Pearrygin 01</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1756,7 +1766,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chewuch River-Doe Creek</t>
+          <t>Chewuch River-Pearrygin Creek</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1764,31 +1774,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Smolt Outmigration</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Entiat River Lake 02</t>
+          <t>Chewuch River Pearrygin 02</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Entiat River-Lake Creek</t>
+          <t>Chewuch River-Pearrygin Creek</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1803,29 +1818,29 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 02</t>
+          <t>Chewuch River Pearrygin 03</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lower Little Wenatchee River</t>
+          <t>Chewuch River-Pearrygin Creek</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1840,19 +1855,19 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 04</t>
+          <t>Chiwawa River Lower 01</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1862,7 +1877,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Lower Little Wenatchee River</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1872,24 +1887,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Adult Migration,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 05</t>
+          <t>Chiwawa River Lower 02</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1899,7 +1914,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lower Little Wenatchee River</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1914,19 +1929,19 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Adult Migration,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Little Wenatchee River Lower 06</t>
+          <t>Chiwawa River Lower 03</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1936,7 +1951,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lower Little Wenatchee River</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1944,21 +1959,26 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Adult Migration,Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 04</t>
+          <t>Chiwawa River Lower 04</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1968,7 +1988,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1978,24 +1998,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 05</t>
+          <t>Chiwawa River Lower 05</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2005,7 +2025,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2015,24 +2035,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Spawning and Incubation,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 06</t>
+          <t>Chiwawa River Lower 06</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2042,7 +2062,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2057,19 +2077,19 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 07</t>
+          <t>Chiwawa River Lower 07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2079,7 +2099,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Chiwawa River</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2094,29 +2114,29 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 15</t>
+          <t>Entiat River Potato 07</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2124,36 +2144,31 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Twisp River Middle 07</t>
+          <t>Entiat River Preston 01</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Middle Twisp River</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2161,36 +2176,31 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Smolt Outmigration</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Antoine 16-1</t>
+          <t>Entiat River Preston 03</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2198,31 +2208,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Antoine 16-2</t>
+          <t>Entiat River Preston 04</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2230,31 +2245,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Antoine 16-3</t>
+          <t>Methow River Thompson 03</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Methow River-Thompson Creek</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2262,31 +2282,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Antoine 16-5</t>
+          <t>Methow River Thompson 05</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Methow River-Thompson Creek</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2294,31 +2319,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Antoine 16-6</t>
+          <t>Methow River Thompson 06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Antoine Creek-Lower</t>
+          <t>Methow River-Thompson Creek</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2326,31 +2356,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Bonaparte 16-1</t>
+          <t>Nason Creek Lower 04</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Bonaparte Creek-Lower DS</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2358,31 +2393,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Loup Loup 16-1</t>
+          <t>Nason Creek Lower 05</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2390,31 +2430,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Loup Loup 16-2</t>
+          <t>Nason Creek Lower 06</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2422,31 +2467,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Loup Loup 16-3</t>
+          <t>Nason Creek Lower 07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Loup Loup Creek-Lower DS</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2454,31 +2504,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Salmon 16-10</t>
+          <t>Nason Creek Lower 15</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2493,29 +2548,29 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Salmon 16-12</t>
+          <t>Entiat River Mills 02</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Entiat River-Mills Creek</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2523,31 +2578,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Salmon 16-2</t>
+          <t>Entiat River Mills 03</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Entiat River-Mills Creek</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2555,31 +2615,36 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Salmon 16-4</t>
+          <t>Entiat River Mills 04</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Entiat River-Mills Creek</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2589,34 +2654,34 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Salmon 16-8</t>
+          <t>Entiat River Mills 06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Entiat River-Mills Creek</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2624,36 +2689,31 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Similkameen 16-2</t>
+          <t>Twisp River Lower 07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Lower Twisp River</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2663,29 +2723,29 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Similkameen 16-3</t>
+          <t>Twisp River Lower 08</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Lower Twisp River</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2693,36 +2753,31 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Similkameen 16-6</t>
+          <t>Twisp River Lower 10</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Similkameen River</t>
+          <t>Lower Twisp River</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2732,29 +2787,29 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Omak 16-2</t>
+          <t>Twisp River Lower 11</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Okanogan</t>
+          <t>Methow</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Lower Twisp River</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2764,19 +2819,19 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Winter Rearing</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Omak 16-3</t>
+          <t>Antoine 16-1</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2786,7 +2841,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2796,19 +2851,19 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Omak 16-5</t>
+          <t>Antoine 16-2</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2818,7 +2873,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2828,19 +2883,19 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Holding and Maturation,Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Omak 16-1</t>
+          <t>Antoine 16-3</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2850,7 +2905,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower DS</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2860,19 +2915,19 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Omak 16-6</t>
+          <t>Antoine 16-5</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2882,7 +2937,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2892,19 +2947,19 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Omak 16-7</t>
+          <t>Antoine 16-6</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2914,7 +2969,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Antoine Creek-Lower</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2924,19 +2979,19 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Omak 16-8</t>
+          <t>Bonaparte 16-1</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2946,7 +3001,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Bonaparte Creek-Lower DS</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2956,19 +3011,19 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Omak 16-9</t>
+          <t>Loup Loup 16-1</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2978,7 +3033,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Omak Creek-Lower US</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2988,19 +3043,19 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Salmon 16-3</t>
+          <t>Loup Loup 16-2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3010,7 +3065,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3020,19 +3075,19 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Salmon 16-7</t>
+          <t>Loup Loup 16-3</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3042,7 +3097,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Salmon Creek-Lower</t>
+          <t>Loup Loup Creek-Lower DS</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3050,36 +3105,31 @@
           <t>Prevent Limiting Factors</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Summer Rearing</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Management and Protection</t>
+          <t>Land Management for Protection</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Twisp River Upper 01</t>
+          <t>Salmon 16-10</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Okanogan</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Upper Twisp River</t>
+          <t>Salmon Creek-Lower</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3094,12 +3144,576 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Spawning and Incubation</t>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Salmon 16-12</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Salmon 16-2</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Salmon 16-4</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Salmon 16-8</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Similkameen 16-2</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Similkameen River</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Similkameen 16-3</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Similkameen River</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Similkameen 16-6</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Similkameen River</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Fry,Holding and Maturation,Summer Rearing,Winter Rearing</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Land Protection (e.g. conservation easement and/or property acquisition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Omak 16-2</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Holding and Maturation,Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Omak 16-3</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Holding and Maturation,Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Omak 16-5</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Holding and Maturation,Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Omak 16-1</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Omak 16-6</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Omak 16-7</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Omak 16-8</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Omak 16-9</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Omak Creek-Lower US</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Salmon 16-3</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Land Management for Protection</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Salmon 16-7</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Okanogan</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Salmon Creek-Lower</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Prevent Limiting Factors</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Summer Rearing</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Land Management for Protection, Land Protection (e.g. conservation easement and/or property acquisition)”</t>
         </is>
       </c>
     </row>

</xml_diff>